<commit_message>
Added "Title" and "Department" to Attendee.  Does not include any Winners Parade changes.
</commit_message>
<xml_diff>
--- a/ATAPS/Content/files/TemplateAttendeeSheet.xlsx
+++ b/ATAPS/Content/files/TemplateAttendeeSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpada\Documents\Visual Studio 2015\Projects\ATAPS\ATAPS\Content\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JosephAdams\Source\Repos\eventand\ATAPS\Content\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="DataFormat" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>LastName</t>
   </si>
@@ -106,6 +106,27 @@
   </si>
   <si>
     <t>String, accepts only UTC8 characters</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>ActivityListNames</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Accounts Payable</t>
+  </si>
+  <si>
+    <t>Welcome Dinner, Universal Studios, Breakout Session 1701</t>
+  </si>
+  <si>
+    <t>String, separated by commas (",") for future parsing</t>
   </si>
 </sst>
 </file>
@@ -477,30 +498,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,6 +564,15 @@
       </c>
       <c r="N1" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -552,36 +583,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
+    <col min="10" max="10" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -624,8 +657,17 @@
       <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -668,8 +710,17 @@
       <c r="N4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -677,7 +728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -685,7 +736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -693,7 +744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -701,7 +752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -709,7 +760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -717,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -725,7 +776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -733,7 +784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -741,7 +792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -749,7 +800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -757,7 +808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -765,7 +816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -773,12 +824,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>